<commit_message>
Actualizacion pequeña de la base de datos de patrocinios
</commit_message>
<xml_diff>
--- a/Patrocinio/Base de datos patricinadores V2.xlsx
+++ b/Patrocinio/Base de datos patricinadores V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cirat/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entre\Desktop\FTC-Into_The_Deep\Patrocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68285C38-92BB-2545-B23B-FACB7705E548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB07B717-1362-4A7F-B6AB-6E2B5F7E33E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12460" xr2:uid="{BA4392A7-1F24-0648-8323-50C177A81C55}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA4392A7-1F24-0648-8323-50C177A81C55}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="140">
   <si>
     <t xml:space="preserve">Juan Valdez </t>
   </si>
@@ -528,9 +539,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -568,7 +579,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -674,7 +685,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -816,7 +827,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -827,20 +838,20 @@
   <dimension ref="A1:G109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C105" sqref="C105"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="94.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.296875" customWidth="1"/>
+    <col min="4" max="4" width="21.296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="25.19921875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="94.19921875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>134</v>
       </c>
@@ -863,7 +874,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -883,7 +894,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -904,7 +915,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -928,7 +939,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -949,7 +960,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -973,7 +984,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -997,7 +1008,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1021,7 +1032,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1042,7 +1053,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1063,7 +1074,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1084,7 +1095,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1108,7 +1119,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13">
         <f>+B11+1</f>
         <v>12</v>
@@ -1123,7 +1134,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1144,7 +1155,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1162,7 +1173,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1183,7 +1194,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1195,7 +1206,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1216,7 +1227,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1237,7 +1248,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1246,7 +1257,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1267,7 +1278,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1285,7 +1296,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1303,7 +1314,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1316,7 +1327,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1335,7 +1346,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1348,7 +1359,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1361,7 +1372,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1382,7 +1393,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1395,7 +1406,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1408,7 +1419,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1427,7 +1438,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1442,7 +1453,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1455,7 +1466,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1474,7 +1485,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1489,7 +1500,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1502,7 +1513,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1523,7 +1534,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1544,7 +1555,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1557,7 +1568,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1576,7 +1587,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1595,7 +1606,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1616,7 +1627,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1629,7 +1640,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1642,7 +1653,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1658,7 +1669,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1674,7 +1685,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1690,7 +1701,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1703,7 +1714,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1724,7 +1735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1742,7 +1753,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1758,7 +1769,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1771,7 +1782,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1787,7 +1798,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1808,7 +1819,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1829,7 +1840,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1845,7 +1856,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1861,7 +1872,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1877,7 +1888,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B59">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1893,7 +1904,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B60">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1908,7 +1919,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1923,7 +1934,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B62">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1938,7 +1949,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B63">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1953,7 +1964,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B64">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1968,7 +1979,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B65">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1983,7 +1994,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B66">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1998,7 +2009,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B67">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -2013,7 +2024,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B68">
         <f t="shared" ref="B68:B109" si="1">+B67+1</f>
         <v>67</v>
@@ -2031,7 +2042,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B69">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -2047,7 +2058,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B70">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -2063,7 +2074,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B71">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -2081,7 +2092,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B72">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -2096,7 +2107,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B73">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -2111,7 +2122,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B74">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -2126,7 +2137,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B75">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -2144,7 +2155,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B76">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -2156,7 +2167,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B77">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -2171,7 +2182,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B78">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -2186,7 +2197,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B79">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -2201,7 +2212,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B80">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -2216,7 +2227,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B81">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -2231,7 +2242,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B82">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -2246,7 +2257,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B83">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -2258,7 +2269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B84">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -2273,7 +2284,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B85">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -2288,7 +2299,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B86">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -2301,7 +2312,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B87">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -2316,7 +2327,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
         <v>136</v>
       </c>
@@ -2327,7 +2338,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B89">
         <f>+B87+1</f>
         <v>87</v>
@@ -2342,7 +2353,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B90">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -2357,7 +2368,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B91">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -2372,7 +2383,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B92">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -2381,7 +2392,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B93">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -2393,7 +2404,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B94">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -2414,7 +2425,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B95">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -2430,7 +2441,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B96">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -2445,7 +2456,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B97">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -2458,7 +2469,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B98">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -2474,7 +2485,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B99">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -2490,7 +2501,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B100">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -2506,7 +2517,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B101">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -2522,7 +2533,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B102">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -2537,7 +2548,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B103">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -2553,7 +2564,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B104">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -2569,7 +2580,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B105">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -2582,7 +2593,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B106">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -2591,7 +2602,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B107">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -2612,7 +2623,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B108">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -2624,13 +2635,16 @@
         <v>111</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B109">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
       <c r="C109" t="s">
         <v>106</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion base de datos de patrocionios
</commit_message>
<xml_diff>
--- a/Patrocinio/Base de datos patricinadores V2.xlsx
+++ b/Patrocinio/Base de datos patricinadores V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entre\Desktop\FTC-Into_The_Deep\Patrocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB07B717-1362-4A7F-B6AB-6E2B5F7E33E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC696158-EDD6-43F9-9E49-3EC791EEB82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA4392A7-1F24-0648-8323-50C177A81C55}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="143">
   <si>
     <t xml:space="preserve">Juan Valdez </t>
   </si>
@@ -446,9 +446,6 @@
     <t>No dan patrocinios</t>
   </si>
   <si>
-    <t>ebay Colombia</t>
-  </si>
-  <si>
     <t>Esperando Respuesta</t>
   </si>
   <si>
@@ -456,6 +453,18 @@
   </si>
   <si>
     <t>Dell TECHNOLOGIES</t>
+  </si>
+  <si>
+    <t>Escribir correo a: servicliente@panamericana.com.co</t>
+  </si>
+  <si>
+    <t>Enviar correo a: talentinquiries@ebat.com</t>
+  </si>
+  <si>
+    <t>eBay</t>
+  </si>
+  <si>
+    <t>Enviar la información requerida por Instagram</t>
   </si>
 </sst>
 </file>
@@ -837,9 +846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953E118B-2559-0648-84DD-D994D8679C8A}">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G114" sqref="G114"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1130,6 +1139,9 @@
       <c r="E13" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>135</v>
       </c>
@@ -2020,8 +2032,11 @@
       <c r="E67" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="F67" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G67" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.3">
@@ -2253,8 +2268,11 @@
       <c r="E82" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="F82" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G82" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.3">
@@ -2295,8 +2313,11 @@
       <c r="E85" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="F85" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G85" s="2" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.3">
@@ -2329,13 +2350,16 @@
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="F88" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G88" s="2" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.3">
@@ -2364,6 +2388,9 @@
       <c r="E90" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="F90" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G90" s="2" t="s">
         <v>95</v>
       </c>
@@ -2438,7 +2465,7 @@
         <v>79</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.3">
@@ -2453,7 +2480,7 @@
         <v>79</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.3">
@@ -2482,7 +2509,7 @@
         <v>79</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.3">
@@ -2498,7 +2525,7 @@
         <v>79</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.3">
@@ -2513,8 +2540,11 @@
       <c r="E100" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="F100" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G100" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.3">
@@ -2523,14 +2553,14 @@
         <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.3">
@@ -2545,7 +2575,7 @@
         <v>79</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.3">
@@ -2561,7 +2591,7 @@
         <v>79</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.3">
@@ -2570,14 +2600,14 @@
         <v>102</v>
       </c>
       <c r="C104" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>